<commit_message>
Some changes made to Production Data
</commit_message>
<xml_diff>
--- a/Project Outputs for USB-UART-ISO-CP2102/Manufacturing Data/BOM/Bill of Materials-USB-UART-ISO-CP2102.xlsx
+++ b/Project Outputs for USB-UART-ISO-CP2102/Manufacturing Data/BOM/Bill of Materials-USB-UART-ISO-CP2102.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desktop\Documents\Project Files\Altium\Projects\Project - Devlopment\USB-UART-ISO-CP2102\Project Outputs for USB-UART-ISO-CP2102\Manufacturing Data\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39D7369E-395B-48AC-9CD6-43BB5F0DA858}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2662BB0A-CCB8-4CCC-8683-3AEBC981F6A2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="13290" xr2:uid="{F23A7062-C17C-4DA0-8E53-5BBC59010D98}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="13290" xr2:uid="{769B7173-9E6A-477D-BDB4-D5A072D0C959}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-USB-UART-ISO-" sheetId="1" r:id="rId1"/>
@@ -830,7 +830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F809A286-609E-489B-82AA-7DEB72AF23C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B719035-B343-4629-AA2C-44E550818761}">
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>